<commit_message>
template für datenbank ausgabe
</commit_message>
<xml_diff>
--- a/static/product_barcodes.xlsx
+++ b/static/product_barcodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CelinaT\Documents\DTG-Studium\Semester_4\Theoriephase\Web\GIT\ScannerMarket\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3116D901-FF00-4E39-BBCE-CD5045791A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D550E20-BF91-40BC-A03A-0B8E241091CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="-1875" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="623">
   <si>
     <t>Getränke</t>
   </si>
@@ -318,9 +318,6 @@
     <t>back bröt</t>
   </si>
   <si>
-    <t>aubergine</t>
-  </si>
-  <si>
     <t>linsen</t>
   </si>
   <si>
@@ -526,9 +523,6 @@
   </si>
   <si>
     <t>rahm</t>
-  </si>
-  <si>
-    <t>nuggets</t>
   </si>
   <si>
     <t>knorr</t>
@@ -2230,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2264,37 +2258,37 @@
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>622</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>3</v>
@@ -2376,22 +2370,22 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>42</v>
@@ -2403,13 +2397,13 @@
         <v>63</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>19</v>
@@ -2418,10 +2412,10 @@
         <v>40056050</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>15</v>
@@ -2433,7 +2427,7 @@
         <v>59</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>10</v>
@@ -2450,10 +2444,10 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>39</v>
@@ -2465,37 +2459,37 @@
         <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>89</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>30</v>
@@ -2524,52 +2518,52 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>37</v>
@@ -2587,63 +2581,63 @@
         <v>45</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>85</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>44</v>
@@ -2655,98 +2649,98 @@
         <v>70</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>83</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>95</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1">
         <v>115728</v>
@@ -2758,37 +2752,37 @@
         <v>42382607</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>76</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N8" s="1">
         <v>76106897</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P8" s="1">
         <v>29066728</v>
@@ -2803,24 +2797,24 @@
         <v>87</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X8" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="1">
         <v>20205775</v>
@@ -2829,43 +2823,43 @@
         <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>84</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>77</v>
@@ -2877,75 +2871,75 @@
         <v>88</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>56</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J10" s="1">
-        <v>20259488</v>
+        <v>159</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>86</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>90</v>
@@ -2954,243 +2948,243 @@
         <v>40804002</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="W10" s="2" t="s">
         <v>69</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>91</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>69</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R12" s="1">
         <v>40255729</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="T12" s="1">
-        <v>20702069</v>
+        <v>100</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B14" s="1">
         <v>29011155</v>
@@ -3199,511 +3193,511 @@
         <v>80</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>162</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L16" s="1">
         <v>42399780</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="P16" s="1">
-        <v>29068050</v>
+      <c r="P16" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B17" s="1">
-        <v>20551926</v>
+        <v>349</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>402</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>163</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="T18" s="1">
+        <v>40081588</v>
+      </c>
+      <c r="U18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="V18" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="R19" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T19" s="1">
-        <v>40081588</v>
+        <v>126</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="H20" s="1">
-        <v>20148027</v>
+        <v>363</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>451</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>127</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
@@ -3711,7 +3705,7 @@
         <v>351</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>80</v>
@@ -3720,416 +3714,416 @@
         <v>42203414</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="N21" s="1">
         <v>42094722</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D23" s="1">
         <v>54491069</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="R23" s="1">
         <v>40255675</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>136</v>
+        <v>333</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>283</v>
+        <v>560</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>353</v>
+        <v>390</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>365</v>
+        <v>35</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>162</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L24" s="1">
         <v>42394501</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="R24" s="1">
         <v>40255705</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B25" s="1">
-        <v>20194987</v>
+        <v>391</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>410</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>35</v>
+        <v>365</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>131</v>
+        <v>335</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>564</v>
+        <v>348</v>
+      </c>
+      <c r="T26" s="1">
+        <v>40397658</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
@@ -4137,497 +4131,461 @@
         <v>393</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>366</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J27" s="1">
-        <v>20445928</v>
+        <v>349</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="T27" s="1">
-        <v>40397658</v>
+        <v>370</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>563</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="H28" s="1">
-        <v>20118907</v>
+        <v>367</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" s="1">
-        <v>3635353</v>
+        <v>349</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>455</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>345</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>372</v>
       </c>
       <c r="T28" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="H29" s="1">
+        <v>43115525</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="T29" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="U28" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="U29" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>348</v>
+        <v>377</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="T30" s="1">
-        <v>24000011859</v>
+        <v>392</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>566</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F31" s="1">
         <v>40084701</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="H31" s="1">
-        <v>43115525</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>457</v>
+        <v>365</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="T31" s="1" t="s">
         <v>567</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C32" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>368</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="T32" s="1" t="s">
         <v>568</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="33" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C33" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F33" s="1">
         <v>80177616</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>379</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>395</v>
+        <v>136</v>
       </c>
       <c r="T33" s="1" t="s">
         <v>569</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="34" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C34" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>442</v>
+        <v>215</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="T34" s="1" t="s">
         <v>570</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C35" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>441</v>
+        <v>214</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="T35" s="1" t="s">
         <v>571</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="36" spans="3:22" x14ac:dyDescent="0.3">
@@ -4635,34 +4593,34 @@
         <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>399</v>
+        <v>112</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>572</v>
@@ -4673,34 +4631,34 @@
         <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>121</v>
+        <v>334</v>
       </c>
       <c r="T37" s="1" t="s">
         <v>573</v>
@@ -4711,34 +4669,34 @@
         <v>79</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>113</v>
+        <v>398</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>574</v>
@@ -4746,37 +4704,37 @@
     </row>
     <row r="39" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C39" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>336</v>
+        <v>120</v>
       </c>
       <c r="T39" s="1" t="s">
         <v>575</v>
@@ -4784,134 +4742,122 @@
     </row>
     <row r="40" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="S40" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="T40" s="1" t="s">
-        <v>576</v>
+        <v>534</v>
       </c>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C41" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T41" s="1" t="s">
-        <v>577</v>
+        <v>527</v>
       </c>
     </row>
     <row r="42" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C42" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="43" spans="3:22" x14ac:dyDescent="0.3">
       <c r="E43" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="44" spans="3:22" x14ac:dyDescent="0.3">
       <c r="E44" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>527</v>
+        <v>293</v>
       </c>
     </row>
     <row r="45" spans="3:22" x14ac:dyDescent="0.3">
       <c r="E45" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>295</v>
+        <v>524</v>
       </c>
     </row>
     <row r="46" spans="3:22" x14ac:dyDescent="0.3">
@@ -4919,27 +4865,27 @@
         <v>33</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="47" spans="3:22" x14ac:dyDescent="0.3">
       <c r="E47" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>525</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="3:22" x14ac:dyDescent="0.3">
@@ -4947,125 +4893,119 @@
         <v>33</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>253</v>
+        <v>506</v>
       </c>
     </row>
     <row r="49" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E49" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>384</v>
+        <v>345</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="50" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E50" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="51" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E51" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="52" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E52" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="O52" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>505</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E53" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E54" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E55" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E56" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E57" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E58" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E59" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>